<commit_message>
update to write SAS
</commit_message>
<xml_diff>
--- a/SAS.xlsx
+++ b/SAS.xlsx
@@ -1815,8 +1815,8 @@
   <dimension ref="A1:P98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A99" sqref="A99"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D103" sqref="D103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>